<commit_message>
feat: Refactor MADCS pages and introduce new functionalities
- Commented out the APA MADCS Stops Part page and its related code for future reference.
- Updated APA MADCS Time Part page to enhance time tracking with new fields and improved button functionalities.
- Enhanced APA MADCS Verification Part page by modifying field names and improving validation logic.
- Updated permissions for APA MADCS ADCS User to reflect changes in codeunit access.
- Introduced new table extensions for APA MADCS ADCS User and Manufacturing Setup to manage additional fields and functionalities.
- Enhanced APA MADCS Prod. Order Component table with new fields for better tracking of consumed quantities.
- Updated APA MADCS Pro Order Line Time table to include new fields for operation tracking and time entries.
- Added new field for logging types in APA MADCS User Log table to categorize log entries.
</commit_message>
<xml_diff>
--- a/David.xlsx
+++ b/David.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://apaware-my.sharepoint.com/personal/servicios_apaware_com/Documents/APAWARE/CLIENTES/DIANACASADO/EXTENSIONES/MADCS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{8DC3DACB-4497-4A78-8077-3D4081E683DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{705DD30A-2C3E-41E1-A9EE-77686DFBA4B9}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{8DC3DACB-4497-4A78-8077-3D4081E683DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4ABFAD0-7CAB-4589-8B2A-1E7355CA3B43}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B377E27A-EFF3-4D26-B93E-67AC9B30EE16}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
   <si>
     <t>Producto</t>
   </si>
@@ -126,12 +126,6 @@
     <t>incidencia</t>
   </si>
   <si>
-    <t>fin estado</t>
-  </si>
-  <si>
-    <t>averia</t>
-  </si>
-  <si>
     <t>tipo incidencia</t>
   </si>
   <si>
@@ -186,9 +180,6 @@
     <t>Consumos</t>
   </si>
   <si>
-    <t>Usuario que marca la opcion de averia cierra el resto de tiempos al resto de usuarios y solo apareceria el</t>
-  </si>
-  <si>
     <t>Fijar hora ytrabajo palnta de forma que si se esta fuera del horario de trabajo(ojo este cambia según temporada) se cierran todos los tiempos</t>
   </si>
   <si>
@@ -211,6 +202,60 @@
   </si>
   <si>
     <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Hay dos tipos de avería, bloqueante  y se para todo y otras no bloqueante pero que permiten seguir funcionando</t>
+  </si>
+  <si>
+    <t>Usuario que marca la opcion de averia si es bloqueante cierra el resto de tiempos al resto de usuarios y solo apareceria el</t>
+  </si>
+  <si>
+    <t>boton para averias bloqueantes</t>
+  </si>
+  <si>
+    <t>boton para averias no bloqueantes</t>
+  </si>
+  <si>
+    <t>Avería no bloqueante</t>
+  </si>
+  <si>
+    <t>averia bloqueante</t>
+  </si>
+  <si>
+    <t>averia no bloqueante</t>
+  </si>
+  <si>
+    <t>según el código de paro</t>
+  </si>
+  <si>
+    <t>-&gt;Para mi trabajo activo e imputa los tiempos a la orden</t>
+  </si>
+  <si>
+    <t>Cada vez que se inicia una operación se para la que tenga activa anteriormente</t>
+  </si>
+  <si>
+    <t>parar trabajo</t>
+  </si>
+  <si>
+    <t>Hay que tener algún sistema para indicar que la orden ya puede ser registrada, que está terminada</t>
+  </si>
+  <si>
+    <t>Cantidad pendiente</t>
+  </si>
+  <si>
+    <t>Cantidad fabricada</t>
+  </si>
+  <si>
+    <t>Cantidad a fabricar</t>
+  </si>
+  <si>
+    <t>Dar salida</t>
+  </si>
+  <si>
+    <t>Finalizar orden</t>
+  </si>
+  <si>
+    <t>Al dar a finalizar orden verificar que los consumos están hechos, que los tiempos están imputados, que las salidas están hechas y parar todos los tiempos pendientes y marcar la orden como finalizada</t>
   </si>
 </sst>
 </file>
@@ -282,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -298,6 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210EFAAB-F6C7-4E33-8BBC-338C48821FBB}">
-  <dimension ref="B2:H82"/>
+  <dimension ref="B2:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -723,7 +769,7 @@
   <sheetData>
     <row r="2" spans="2:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C2" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
@@ -767,15 +813,15 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1</v>
@@ -787,7 +833,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
@@ -819,7 +865,7 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.2">
@@ -849,22 +895,22 @@
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="3:8" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C27" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -906,7 +952,7 @@
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C43" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.2">
@@ -933,7 +979,7 @@
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>1</v>
@@ -958,22 +1004,22 @@
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C54" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C55" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C56" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C57" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.2">
@@ -996,7 +1042,7 @@
         <v>23</v>
       </c>
       <c r="F63" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="3:8" x14ac:dyDescent="0.2">
@@ -1007,7 +1053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D65">
         <v>15</v>
       </c>
@@ -1015,7 +1061,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E66" t="s">
+        <v>59</v>
+      </c>
+      <c r="F66" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C68" s="4" t="s">
         <v>25</v>
       </c>
@@ -1026,42 +1080,113 @@
         <v>27</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D71" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C74" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="75" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="77" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
-        <v>50</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C78" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="80" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C80" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="81" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C81" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="82" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C82" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="D82" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F82" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C83" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="89" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C89" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F89" s="6"/>
+    </row>
+    <row r="90" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90" t="s">
+        <v>69</v>
+      </c>
+      <c r="E90" t="s">
+        <v>68</v>
+      </c>
+      <c r="F90" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="92" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C92" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="94" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C94" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="95" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C95" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="C89:F89"/>
     <mergeCell ref="C27:F27"/>
     <mergeCell ref="C62:F62"/>
     <mergeCell ref="C2:H2"/>
@@ -1070,7 +1195,7 @@
     <mergeCell ref="D23:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -1087,10 +1212,10 @@
   <sheetData>
     <row r="14" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="4:6" x14ac:dyDescent="0.2">
@@ -1098,7 +1223,7 @@
         <v>10024</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F15">
         <v>10</v>
@@ -1106,12 +1231,12 @@
     </row>
     <row r="16" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.2">

</xml_diff>